<commit_message>
Added more tests for period_fun.
</commit_message>
<xml_diff>
--- a/pkg/tests/testthat/read_ts/xlsx/example3.xlsx
+++ b/pkg/tests/testthat/read_ts/xlsx/example3.xlsx
@@ -28,16 +28,16 @@
     <t xml:space="preserve">b</t>
   </si>
   <si>
-    <t xml:space="preserve">2010Q2</t>
+    <t xml:space="preserve">april 2010</t>
   </si>
   <si>
     <t xml:space="preserve">NOTE: We have no other data for  2010</t>
   </si>
   <si>
-    <t xml:space="preserve">2011Q1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2011Q2</t>
+    <t xml:space="preserve">january 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">april 2011</t>
   </si>
   <si>
     <t xml:space="preserve">xxxxx</t>
@@ -50,8 +50,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -118,8 +119,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -143,19 +148,19 @@
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14:C15"/>
+      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -167,7 +172,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -183,7 +188,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="0" t="n">

</xml_diff>